<commit_message>
billing keyword and page object update
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/billing_test_data.xlsx
+++ b/TestData/Web_POS/Billing/billing_test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95" count="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="97" count="716">
   <si>
     <t>TC_Id</t>
   </si>
@@ -299,6 +299,12 @@
   </si>
   <si>
     <t>Remark</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>Dummy</t>
   </si>
 </sst>
 </file>
@@ -628,7 +634,7 @@
   <sheetPr>
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:X45"/>
+  <dimension ref="A1:Y45"/>
   <sheetViews>
     <sheetView view="normal" tabSelected="1" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" sqref="C8"/>
@@ -653,7 +659,7 @@
     <col min="23" max="23" width="18.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" customHeight="1">
+    <row r="1" spans="1:25" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -726,8 +732,11 @@
       <c r="X1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="33.75" customHeight="1">
+      <c r="Y1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="33.75" customHeight="1">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -788,8 +797,11 @@
       <c r="T2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" ht="33.75" customHeight="1">
+      <c r="Y2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" ht="33.75" customHeight="1">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -850,8 +862,11 @@
       <c r="T3" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" ht="33.75" customHeight="1">
+      <c r="Y3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" ht="33.75" customHeight="1">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -912,8 +927,11 @@
       <c r="T4" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="45" customHeight="1">
+      <c r="Y4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="45" customHeight="1">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -974,8 +992,11 @@
       <c r="T5" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" ht="19.5" customHeight="1">
+      <c r="Y5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="19.5" customHeight="1">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1036,8 +1057,11 @@
       <c r="T6" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" customHeight="1">
+      <c r="Y6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" customHeight="1">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1098,8 +1122,11 @@
       <c r="T7" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" ht="26.25" customHeight="1">
+      <c r="Y7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="26.25" customHeight="1">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1160,8 +1187,11 @@
       <c r="T8" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" ht="30" customHeight="1">
+      <c r="Y8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="30" customHeight="1">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1222,8 +1252,11 @@
       <c r="T9" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" ht="31.5" customHeight="1">
+      <c r="Y9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="31.5" customHeight="1">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1284,8 +1317,11 @@
       <c r="T10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" ht="32.25" customHeight="1">
+      <c r="Y10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="32.25" customHeight="1">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1346,8 +1382,11 @@
       <c r="T11" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" ht="28.5" customHeight="1">
+      <c r="Y11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="28.5" customHeight="1">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1408,8 +1447,11 @@
       <c r="T12" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" ht="14.25">
+      <c r="Y12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="24">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1470,8 +1512,11 @@
       <c r="T13" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" ht="14.25">
+      <c r="Y13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="24">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1532,8 +1577,11 @@
       <c r="T14" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" ht="14.25">
+      <c r="Y14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="24">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1594,8 +1642,11 @@
       <c r="T15" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" ht="14.25">
+      <c r="Y15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="24">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -1656,8 +1707,11 @@
       <c r="T16" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" ht="14.25">
+      <c r="Y16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="24">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1718,8 +1772,11 @@
       <c r="T17" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" ht="14.25">
+      <c r="Y17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="24">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1780,8 +1837,11 @@
       <c r="T18" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" ht="14.25">
+      <c r="Y18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="24">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -1842,8 +1902,11 @@
       <c r="T19" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" ht="14.25">
+      <c r="Y19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" ht="24">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -1904,8 +1967,11 @@
       <c r="T20" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" ht="14.25">
+      <c r="Y20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="24">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -1966,8 +2032,11 @@
       <c r="T21" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" ht="14.25">
+      <c r="Y21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" ht="24">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -2028,9 +2097,16 @@
       <c r="T22" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" ht="15"/>
-    <row r="24" spans="1:24">
+      <c r="Y22" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="25:25">
+      <c r="Y23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -2099,8 +2175,11 @@
       <c r="X24" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:24">
+      <c r="Y24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -2169,8 +2248,11 @@
       <c r="X25" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:24">
+      <c r="Y25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -2239,8 +2321,11 @@
       <c r="X26" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:24">
+      <c r="Y26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -2306,8 +2391,11 @@
       <c r="X27" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="28" spans="1:24">
+      <c r="Y27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -2376,8 +2464,11 @@
       <c r="X28" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:24">
+      <c r="Y28" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -2446,8 +2537,11 @@
       <c r="X29" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:24">
+      <c r="Y29" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25">
       <c r="A30" t="s">
         <v>72</v>
       </c>
@@ -2516,8 +2610,11 @@
       <c r="X30" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:24">
+      <c r="Y30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -2586,8 +2683,11 @@
       <c r="X31" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="32" spans="1:24">
+      <c r="Y31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -2656,8 +2756,11 @@
       <c r="X32" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:24">
+      <c r="Y32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -2726,8 +2829,11 @@
       <c r="X33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:24">
+      <c r="Y33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25">
       <c r="A34" t="s">
         <v>78</v>
       </c>
@@ -2796,8 +2902,11 @@
       <c r="X34" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="1:24">
+      <c r="Y34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -2866,8 +2975,11 @@
       <c r="X35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:24">
+      <c r="Y35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -2936,8 +3048,11 @@
       <c r="X36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:24">
+      <c r="Y36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -3006,8 +3121,11 @@
       <c r="X37" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:24">
+      <c r="Y37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -3076,8 +3194,11 @@
       <c r="X38" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:24">
+      <c r="Y38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -3146,8 +3267,11 @@
       <c r="X39" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="40" spans="1:24">
+      <c r="Y39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -3216,8 +3340,11 @@
       <c r="X40" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="41" spans="1:24">
+      <c r="Y40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -3286,8 +3413,11 @@
       <c r="X41" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="42" spans="1:24">
+      <c r="Y41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -3356,8 +3486,11 @@
       <c r="X42" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="43" spans="1:24">
+      <c r="Y42" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25">
       <c r="A43" t="s">
         <v>88</v>
       </c>
@@ -3426,8 +3559,11 @@
       <c r="X43" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="44" spans="1:24">
+      <c r="Y43" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -3496,8 +3632,11 @@
       <c r="X44" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="45" spans="1:24">
+      <c r="Y44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25">
       <c r="A45" t="s">
         <v>90</v>
       </c>
@@ -3565,6 +3704,9 @@
       </c>
       <c r="X45" t="s">
         <v>35</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>